<commit_message>
update PDF, and update excel to match document
</commit_message>
<xml_diff>
--- a/logistics/teamSprintSheet-Group6.xlsx
+++ b/logistics/teamSprintSheet-Group6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anahita/Documents/U/U2016/UIC/Term 6/CS 342/Project 5 2/Group 6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ttcttctwAtGDrive\Keep On Cloud\UIC 2019 Spring\CS 342\CS 342-Project 5\cs342_project5\logistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68ABD5A1-3FA3-7F4A-BF89-C70B5FF53F63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FDE079-9498-4CBB-BE38-0FDBF305CD49}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" xr2:uid="{295B521D-40CD-0741-A7F0-C29826591B86}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{295B521D-40CD-0741-A7F0-C29826591B86}"/>
   </bookViews>
   <sheets>
     <sheet name="April 1" sheetId="2" r:id="rId1"/>
@@ -77,47 +77,47 @@
     <t xml:space="preserve">Client and server communication with Arshad, client gui using react </t>
   </si>
   <si>
-    <t>continuing working on client gui using react</t>
-  </si>
-  <si>
     <t>Jigar</t>
   </si>
   <si>
     <t>Server backend (communication and logic)</t>
   </si>
   <si>
-    <t>inetgration of the server component to other components such client gui</t>
-  </si>
-  <si>
     <t>Arshad</t>
   </si>
   <si>
     <t>Setup react and established communication between server and client that uses react</t>
   </si>
   <si>
-    <t>proper display of evaluation of server on client gui (communication from server to client), socket.io for client</t>
-  </si>
-  <si>
     <t>Angela</t>
   </si>
   <si>
     <t>creating classes on server side (game logic) and storing data</t>
   </si>
   <si>
-    <t>Testing that game logic works, integration of game logic to other components with Jigar</t>
-  </si>
-  <si>
     <t>Final Project Documentation</t>
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>Client UI and server-side testing + project documentation (This doc, and README)</t>
+  </si>
+  <si>
+    <t>Server – NodeJS Server &amp; Client communication via strings &amp; accept multiple clients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client &amp; Server – Set up client-side w/ React &amp; establish connection w/ NodeJS </t>
+  </si>
+  <si>
+    <t>Server – Front end keyboard input and classes for server side</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -153,6 +153,13 @@
       <color theme="1"/>
       <name val="Gill Sans MT"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -452,23 +459,23 @@
   </sheetPr>
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="173" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" thickBottom="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="22.2" thickBottom="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="53" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="36.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="41.296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.296875" style="1" customWidth="1"/>
     <col min="6" max="6" width="38.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="42.83203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="42.796875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="30" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
@@ -479,27 +486,27 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="30" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="30" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="30" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="30" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="30" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:7" s="7" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="7" customFormat="1" ht="54" x14ac:dyDescent="0.5">
       <c r="A7" s="7" t="s">
         <v>0</v>
       </c>
@@ -522,8 +529,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="6" customFormat="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:7" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="6" customFormat="1" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="9" spans="1:7" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="8">
         <v>1</v>
       </c>
@@ -534,114 +541,115 @@
         <v>13</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="8">
         <v>2</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>16</v>
-      </c>
       <c r="F10" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="8">
         <v>3</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="8">
         <v>4</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B13" s="8">
         <v>5</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:7" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:7" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="4:5" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="4:5" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="4:5" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="4:5" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="4:5" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="4:5" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="4:5" s="6" customFormat="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="4:5" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="15" spans="1:7" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="16" spans="1:7" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="17" spans="4:5" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="18" spans="4:5" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="19" spans="4:5" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="20" spans="4:5" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="21" spans="4:5" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="22" spans="4:5" s="8" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="23" spans="4:5" s="6" customFormat="1" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="32" spans="4:5" ht="30" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D32" s="5"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="4:5" ht="24" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D33" s="3"/>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="4:5" ht="24" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D34" s="3"/>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="4:5" ht="24" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D35" s="3"/>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="4:5" ht="24" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D36" s="3"/>
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="4:5" ht="24" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D37" s="3"/>
       <c r="E37" s="4"/>
     </row>
-    <row r="38" spans="4:5" ht="24" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D38" s="3"/>
       <c r="E38" s="4"/>
     </row>
-    <row r="39" spans="4:5" ht="24" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D39" s="3"/>
       <c r="E39" s="4"/>
     </row>
-    <row r="40" spans="4:5" ht="24" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
     </row>
-    <row r="41" spans="4:5" ht="24" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="46" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="46" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>